<commit_message>
Added file save and text file compare tests
</commit_message>
<xml_diff>
--- a/Test/RevitKeynotes_Imperial.xlsx
+++ b/Test/RevitKeynotes_Imperial.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RevitKeynotes_Imperial" sheetId="1" r:id="rId1"/>
@@ -28554,7 +28554,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -29389,12 +29389,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5053"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="50.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">

</xml_diff>